<commit_message>
FigS7B and S18A added
</commit_message>
<xml_diff>
--- a/figures/Fig3C.xlsx
+++ b/figures/Fig3C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10321"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junyao/Desktop/tempFLEXI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junyao/Documents/NGS/full_length_intron/Paper/FLEXI_git/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E2A0CA-4FF4-D345-A296-BBD1093DC60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85D001B-7101-A541-9F55-36F6FCA3CA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{BA43CD70-9CD1-CA49-8179-2E1358CD31BA}"/>
+    <workbookView xWindow="-29420" yWindow="2220" windowWidth="28040" windowHeight="17440" xr2:uid="{BA43CD70-9CD1-CA49-8179-2E1358CD31BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>&lt;0.75FLEXI</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Protein coding</t>
+  </si>
+  <si>
+    <t>&lt;0.25FLEXI</t>
+  </si>
+  <si>
+    <t>&lt;0.50FLEXI</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76356014-3B7C-8749-95F6-E5A31025E921}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,254 +490,390 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B2">
-        <v>7940</v>
+        <v>6821</v>
       </c>
       <c r="C2">
-        <v>7673</v>
+        <v>6583</v>
       </c>
       <c r="D2">
-        <v>1984</v>
+        <v>1667</v>
       </c>
       <c r="E2">
-        <v>2788</v>
+        <v>2270</v>
       </c>
       <c r="F2">
-        <v>1450</v>
+        <v>1168</v>
       </c>
       <c r="G2">
-        <v>616</v>
+        <v>516</v>
       </c>
       <c r="I2" s="2">
-        <f>C2/($B2)</f>
-        <v>0.96637279596977332</v>
+        <f t="shared" ref="I2:I3" si="0">C2/($B2)</f>
+        <v>0.96510775546107608</v>
       </c>
       <c r="J2" s="2">
-        <f t="shared" ref="J2:M4" si="0">D2/($B2)</f>
-        <v>0.24987405541561714</v>
+        <f t="shared" ref="J2:J3" si="1">D2/($B2)</f>
+        <v>0.24439231784195867</v>
       </c>
       <c r="K2" s="2">
-        <f t="shared" si="0"/>
-        <v>0.35113350125944587</v>
+        <f t="shared" ref="K2:K3" si="2">E2/($B2)</f>
+        <v>0.33279577774519864</v>
       </c>
       <c r="L2" s="2">
-        <f t="shared" si="0"/>
-        <v>0.18261964735516373</v>
+        <f t="shared" ref="L2:L3" si="3">F2/($B2)</f>
+        <v>0.17123588916581148</v>
       </c>
       <c r="M2" s="2">
-        <f t="shared" si="0"/>
-        <v>7.758186397984887E-2</v>
+        <f t="shared" ref="M2:M3" si="4">G2/($B2)</f>
+        <v>7.5648731857498902E-2</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>158</v>
+        <v>7731</v>
       </c>
       <c r="C3">
-        <v>154</v>
+        <v>7468</v>
       </c>
       <c r="D3">
-        <v>75</v>
+        <v>1917</v>
       </c>
       <c r="E3">
-        <v>109</v>
+        <v>2667</v>
       </c>
       <c r="F3">
-        <v>70</v>
+        <v>1377</v>
       </c>
       <c r="G3">
-        <v>32</v>
+        <v>589</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I4" si="1">C3/($B3)</f>
-        <v>0.97468354430379744</v>
+        <f t="shared" si="0"/>
+        <v>0.96598111499159234</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" si="0"/>
-        <v>0.47468354430379744</v>
+        <f t="shared" si="1"/>
+        <v>0.2479627473806752</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" si="0"/>
-        <v>0.689873417721519</v>
+        <f t="shared" si="2"/>
+        <v>0.34497477687233219</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" si="0"/>
-        <v>0.44303797468354428</v>
+        <f t="shared" si="3"/>
+        <v>0.1781140861466822</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" si="0"/>
-        <v>0.20253164556962025</v>
+        <f t="shared" si="4"/>
+        <v>7.6186780494114606E-2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>7940</v>
+      </c>
+      <c r="C4">
+        <v>7673</v>
+      </c>
+      <c r="D4">
+        <v>1984</v>
+      </c>
+      <c r="E4">
+        <v>2788</v>
+      </c>
+      <c r="F4">
+        <v>1450</v>
+      </c>
+      <c r="G4">
+        <v>616</v>
+      </c>
+      <c r="I4" s="2">
+        <f>C4/($B4)</f>
+        <v>0.96637279596977332</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:M6" si="5">D4/($B4)</f>
+        <v>0.24987405541561714</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" si="5"/>
+        <v>0.35113350125944587</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" si="5"/>
+        <v>0.18261964735516373</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" si="5"/>
+        <v>7.758186397984887E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>158</v>
+      </c>
+      <c r="C5">
+        <v>154</v>
+      </c>
+      <c r="D5">
+        <v>75</v>
+      </c>
+      <c r="E5">
+        <v>109</v>
+      </c>
+      <c r="F5">
+        <v>70</v>
+      </c>
+      <c r="G5">
+        <v>32</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" ref="I5:I6" si="6">C5/($B5)</f>
+        <v>0.97468354430379744</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="5"/>
+        <v>0.47468354430379744</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="5"/>
+        <v>0.689873417721519</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="5"/>
+        <v>0.44303797468354428</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="5"/>
+        <v>0.20253164556962025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>44</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>44</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>29</v>
       </c>
-      <c r="E4">
+      <c r="E6">
         <v>34</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <v>31</v>
       </c>
-      <c r="G4">
+      <c r="G6">
         <v>13</v>
       </c>
-      <c r="I4" s="2">
-        <f t="shared" si="1"/>
+      <c r="I6" s="2">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="J4" s="2">
-        <f t="shared" si="0"/>
+      <c r="J6" s="2">
+        <f t="shared" si="5"/>
         <v>0.65909090909090906</v>
       </c>
-      <c r="K4" s="2">
-        <f t="shared" si="0"/>
+      <c r="K6" s="2">
+        <f t="shared" si="5"/>
         <v>0.77272727272727271</v>
       </c>
-      <c r="L4" s="2">
-        <f t="shared" si="0"/>
+      <c r="L6" s="2">
+        <f t="shared" si="5"/>
         <v>0.70454545454545459</v>
       </c>
-      <c r="M4" s="2">
-        <f t="shared" si="0"/>
+      <c r="M6" s="2">
+        <f t="shared" si="5"/>
         <v>0.29545454545454547</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>5</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E16" t="s">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F16" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="3" t="str">
-        <f>C2&amp;" ("&amp;ROUND(100*I2,1)&amp;"%)"</f>
-        <v>7673 (96.6%)</v>
-      </c>
-      <c r="C15" s="3" t="str">
-        <f t="shared" ref="C15:D17" si="2">E2&amp;" ("&amp;ROUND(100*K2,1)&amp;"%)"</f>
-        <v>2788 (35.1%)</v>
-      </c>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>1450 (18.3%)</v>
-      </c>
-      <c r="E15" s="3" t="str">
-        <f>D2&amp;" ("&amp;ROUND(100*J2,1)&amp;"%)"</f>
-        <v>1984 (25%)</v>
-      </c>
-      <c r="F15" s="3" t="str">
-        <f>G2&amp;" ("&amp;ROUND(100*M2,1)&amp;"%)"</f>
-        <v>616 (7.8%)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="str">
-        <f t="shared" ref="B16" si="3">C3&amp;" ("&amp;ROUND(100*I3,1)&amp;"%)"</f>
-        <v>154 (97.5%)</v>
-      </c>
-      <c r="C16" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>109 (69%)</v>
-      </c>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>70 (44.3%)</v>
-      </c>
-      <c r="E16" s="3" t="str">
-        <f>D3&amp;" ("&amp;ROUND(100*J3,1)&amp;"%)"</f>
-        <v>75 (47.5%)</v>
-      </c>
-      <c r="F16" s="3" t="str">
-        <f>G3&amp;" ("&amp;ROUND(100*M3,1)&amp;"%)"</f>
-        <v>32 (20.3%)</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f t="shared" ref="B17:B18" si="7">C2&amp;" ("&amp;ROUND(100*I2,1)&amp;"%)"</f>
+        <v>6583 (96.5%)</v>
+      </c>
+      <c r="C17" s="3" t="str">
+        <f t="shared" ref="C17:C18" si="8">E2&amp;" ("&amp;ROUND(100*K2,1)&amp;"%)"</f>
+        <v>2270 (33.3%)</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" ref="D17:D18" si="9">F2&amp;" ("&amp;ROUND(100*L2,1)&amp;"%)"</f>
+        <v>1168 (17.1%)</v>
+      </c>
+      <c r="E17" s="3" t="str">
+        <f t="shared" ref="E17:E18" si="10">D2&amp;" ("&amp;ROUND(100*J2,1)&amp;"%)"</f>
+        <v>1667 (24.4%)</v>
+      </c>
+      <c r="F17" s="3" t="str">
+        <f t="shared" ref="F17:F18" si="11">G2&amp;" ("&amp;ROUND(100*M2,1)&amp;"%)"</f>
+        <v>516 (7.6%)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>7468 (96.6%)</v>
+      </c>
+      <c r="C18" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>2667 (34.5%)</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>1377 (17.8%)</v>
+      </c>
+      <c r="E18" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>1917 (24.8%)</v>
+      </c>
+      <c r="F18" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>589 (7.6%)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="3" t="str">
+        <f>C4&amp;" ("&amp;ROUND(100*I4,1)&amp;"%)"</f>
+        <v>7673 (96.6%)</v>
+      </c>
+      <c r="C19" s="3" t="str">
+        <f t="shared" ref="C19:D21" si="12">E4&amp;" ("&amp;ROUND(100*K4,1)&amp;"%)"</f>
+        <v>2788 (35.1%)</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>1450 (18.3%)</v>
+      </c>
+      <c r="E19" s="3" t="str">
+        <f>D4&amp;" ("&amp;ROUND(100*J4,1)&amp;"%)"</f>
+        <v>1984 (25%)</v>
+      </c>
+      <c r="F19" s="3" t="str">
+        <f>G4&amp;" ("&amp;ROUND(100*M4,1)&amp;"%)"</f>
+        <v>616 (7.8%)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="str">
+        <f t="shared" ref="B20" si="13">C5&amp;" ("&amp;ROUND(100*I5,1)&amp;"%)"</f>
+        <v>154 (97.5%)</v>
+      </c>
+      <c r="C20" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>109 (69%)</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>70 (44.3%)</v>
+      </c>
+      <c r="E20" s="3" t="str">
+        <f>D5&amp;" ("&amp;ROUND(100*J5,1)&amp;"%)"</f>
+        <v>75 (47.5%)</v>
+      </c>
+      <c r="F20" s="3" t="str">
+        <f>G5&amp;" ("&amp;ROUND(100*M5,1)&amp;"%)"</f>
+        <v>32 (20.3%)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="3" t="str">
-        <f t="shared" ref="B17" si="4">C4&amp;" ("&amp;ROUND(100*I4,1)&amp;"%)"</f>
+      <c r="B21" s="3" t="str">
+        <f t="shared" ref="B21" si="14">C6&amp;" ("&amp;ROUND(100*I6,1)&amp;"%)"</f>
         <v>44 (100%)</v>
       </c>
-      <c r="C17" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="C21" s="3" t="str">
+        <f t="shared" si="12"/>
         <v>34 (77.3%)</v>
       </c>
-      <c r="D17" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="12"/>
         <v>31 (70.5%)</v>
       </c>
-      <c r="E17" s="3" t="str">
-        <f>D4&amp;" ("&amp;ROUND(100*J4,1)&amp;"%)"</f>
+      <c r="E21" s="3" t="str">
+        <f>D6&amp;" ("&amp;ROUND(100*J6,1)&amp;"%)"</f>
         <v>29 (65.9%)</v>
       </c>
-      <c r="F17" s="3" t="str">
-        <f>G4&amp;" ("&amp;ROUND(100*M4,1)&amp;"%)"</f>
+      <c r="F21" s="3" t="str">
+        <f>G6&amp;" ("&amp;ROUND(100*M6,1)&amp;"%)"</f>
         <v>13 (29.5%)</v>
       </c>
     </row>

</xml_diff>